<commit_message>
Updated ETL and uploaded latest transactions
</commit_message>
<xml_diff>
--- a/source files/budget_jodine.xlsx
+++ b/source files/budget_jodine.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jay/GIT Repos/ftrack/source files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{281BFA3C-362E-4441-85DB-B432EEF117C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C81A9A48-D1B0-1346-AA3A-EEC17EFF6123}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-68800" yWindow="-5900" windowWidth="68800" windowHeight="28300" xr2:uid="{F25DD163-696E-F842-A897-5E899A2812A7}"/>
+    <workbookView xWindow="-49100" yWindow="-5900" windowWidth="68800" windowHeight="28300" activeTab="1" xr2:uid="{F25DD163-696E-F842-A897-5E899A2812A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Jodine Transactional" sheetId="24" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="33">
   <si>
     <t>Jeanre Transactional</t>
   </si>
@@ -124,6 +124,21 @@
   </si>
   <si>
     <t>Vape</t>
+  </si>
+  <si>
+    <t>Budget Retained Balance</t>
+  </si>
+  <si>
+    <t>Eating Out</t>
+  </si>
+  <si>
+    <t>Deneysville Visit</t>
+  </si>
+  <si>
+    <t>Jeanre Cash</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -786,151 +801,343 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="16"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
+        <color auto="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color auto="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color auto="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color auto="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color auto="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color auto="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color auto="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color auto="1"/>
         <name val="Aptos Narrow"/>
         <scheme val="minor"/>
       </font>
@@ -968,6 +1175,25 @@
     </dxf>
     <dxf>
       <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color auto="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -981,217 +1207,6 @@
         <color theme="1"/>
         <name val="Aptos Narrow"/>
         <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color auto="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color auto="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color auto="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color auto="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color auto="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color auto="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color auto="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color auto="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color auto="1"/>
-        <name val="Aptos Narrow"/>
         <scheme val="minor"/>
       </font>
       <fill>
@@ -1302,151 +1317,343 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="16"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
+        <color auto="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color auto="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color auto="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color auto="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color auto="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color auto="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color auto="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color auto="1"/>
         <name val="Aptos Narrow"/>
         <scheme val="minor"/>
       </font>
@@ -1484,6 +1691,25 @@
     </dxf>
     <dxf>
       <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color auto="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -1497,217 +1723,6 @@
         <color theme="1"/>
         <name val="Aptos Narrow"/>
         <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color auto="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color auto="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color auto="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color auto="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color auto="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color auto="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color auto="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color auto="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color auto="1"/>
-        <name val="Aptos Narrow"/>
         <scheme val="minor"/>
       </font>
       <fill>
@@ -1818,151 +1833,343 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="16"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
+        <color auto="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color auto="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color auto="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color auto="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color auto="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color auto="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color auto="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color auto="1"/>
         <name val="Aptos Narrow"/>
         <scheme val="minor"/>
       </font>
@@ -2000,6 +2207,25 @@
     </dxf>
     <dxf>
       <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color auto="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -2013,217 +2239,6 @@
         <color theme="1"/>
         <name val="Aptos Narrow"/>
         <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color auto="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color auto="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color auto="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color auto="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color auto="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color auto="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color auto="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color auto="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color auto="1"/>
-        <name val="Aptos Narrow"/>
         <scheme val="minor"/>
       </font>
       <fill>
@@ -2867,30 +2882,30 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{586FC7B9-BD4A-294C-BAE6-F476073EB80A}" name="Table327" displayName="Table327" ref="A1:J11" totalsRowCount="1" headerRowDxfId="109" dataDxfId="108">
   <autoFilter ref="A1:J10" xr:uid="{92565AF6-51CB-F740-ACD0-AD376C5F8FE0}"/>
   <tableColumns count="10">
-    <tableColumn id="5" xr3:uid="{6E69B458-4FF6-AA41-95BC-EDC678BC0093}" name="Movement" totalsRowLabel="Subtotal" dataDxfId="107" totalsRowDxfId="9"/>
-    <tableColumn id="6" xr3:uid="{D47E3C5D-B818-7F4B-BFEC-DDA7481F4587}" name="Account Secondary" totalsRowLabel="Jodine Transactional" dataDxfId="106" totalsRowDxfId="8"/>
-    <tableColumn id="7" xr3:uid="{A673DCA8-3181-2B48-A287-B7DC290508A8}" name="2024-05-01" totalsRowFunction="custom" dataDxfId="105" totalsRowDxfId="7">
+    <tableColumn id="5" xr3:uid="{6E69B458-4FF6-AA41-95BC-EDC678BC0093}" name="Movement" totalsRowLabel="Subtotal" dataDxfId="107" totalsRowDxfId="19"/>
+    <tableColumn id="6" xr3:uid="{D47E3C5D-B818-7F4B-BFEC-DDA7481F4587}" name="Account Secondary" totalsRowLabel="Jodine Transactional" dataDxfId="106" totalsRowDxfId="18"/>
+    <tableColumn id="7" xr3:uid="{A673DCA8-3181-2B48-A287-B7DC290508A8}" name="2024-05-01" totalsRowFunction="custom" dataDxfId="105" totalsRowDxfId="17">
       <totalsRowFormula>SUMIF(Table327[[#Data],[#Totals],[Movement]],"Credit", Table327[[#Data],[#Totals],[2024-05-01]])-SUMIF(Table327[[#Data],[#Totals],[Movement]],"Debit", Table327[[#Data],[#Totals],[2024-05-01]])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{B6E7D547-5D0E-6D41-8F04-8C1F455CCAC3}" name="2024-06-01" totalsRowFunction="custom" dataDxfId="104" totalsRowDxfId="6">
+    <tableColumn id="8" xr3:uid="{B6E7D547-5D0E-6D41-8F04-8C1F455CCAC3}" name="2024-06-01" totalsRowFunction="custom" dataDxfId="104" totalsRowDxfId="16">
       <totalsRowFormula>SUMIF(Table327[[#Data],[#Totals],[Movement]],"Credit", Table327[[#Data],[#Totals],[2024-06-01]])-SUMIF(Table327[[#Data],[#Totals],[Movement]],"Debit", Table327[[#Data],[#Totals],[2024-06-01]])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{EED6F578-2107-254B-B19B-3613DFC61464}" name="2024-07-01" totalsRowFunction="custom" dataDxfId="103" totalsRowDxfId="5">
+    <tableColumn id="9" xr3:uid="{EED6F578-2107-254B-B19B-3613DFC61464}" name="2024-07-01" totalsRowFunction="custom" dataDxfId="103" totalsRowDxfId="15">
       <totalsRowFormula>SUMIF(Table327[[#Data],[#Totals],[Movement]],"Credit", Table327[[#Data],[#Totals],[2024-07-01]])-SUMIF(Table327[[#Data],[#Totals],[Movement]],"Debit", Table327[[#Data],[#Totals],[2024-07-01]])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{C2FA8C69-9A64-764E-B91D-232CF4696276}" name="2024-08-01" totalsRowFunction="custom" dataDxfId="102" totalsRowDxfId="4">
+    <tableColumn id="10" xr3:uid="{C2FA8C69-9A64-764E-B91D-232CF4696276}" name="2024-08-01" totalsRowFunction="custom" dataDxfId="102" totalsRowDxfId="14">
       <totalsRowFormula>SUMIF(Table327[[#Data],[#Totals],[Movement]],"Credit", Table327[[#Data],[#Totals],[2024-08-01]])-SUMIF(Table327[[#Data],[#Totals],[Movement]],"Debit", Table327[[#Data],[#Totals],[2024-08-01]])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{DA8F87DE-6FA5-C542-A1E2-C65545DB76F6}" name="2024-09-01" totalsRowFunction="custom" dataDxfId="101" totalsRowDxfId="3">
+    <tableColumn id="11" xr3:uid="{DA8F87DE-6FA5-C542-A1E2-C65545DB76F6}" name="2024-09-01" totalsRowFunction="custom" dataDxfId="101" totalsRowDxfId="13">
       <totalsRowFormula>SUMIF(Table327[[#Data],[#Totals],[Movement]],"Credit", Table327[[#Data],[#Totals],[2024-09-01]])-SUMIF(Table327[[#Data],[#Totals],[Movement]],"Debit", Table327[[#Data],[#Totals],[2024-09-01]])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{2744F012-CFCA-FC43-8A49-88A121FA14CE}" name="2024-10-01" totalsRowFunction="custom" dataDxfId="100" totalsRowDxfId="2">
+    <tableColumn id="12" xr3:uid="{2744F012-CFCA-FC43-8A49-88A121FA14CE}" name="2024-10-01" totalsRowFunction="custom" dataDxfId="100" totalsRowDxfId="12">
       <totalsRowFormula>SUMIF(Table327[[#Data],[#Totals],[Movement]],"Credit", Table327[[#Data],[#Totals],[2024-10-01]])-SUMIF(Table327[[#Data],[#Totals],[Movement]],"Debit", Table327[[#Data],[#Totals],[2024-10-01]])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{39FF230A-B9E3-3242-ABFB-EB1A480E6CB3}" name="2024-11-01" totalsRowFunction="custom" dataDxfId="99" totalsRowDxfId="1">
+    <tableColumn id="13" xr3:uid="{39FF230A-B9E3-3242-ABFB-EB1A480E6CB3}" name="2024-11-01" totalsRowFunction="custom" dataDxfId="99" totalsRowDxfId="11">
       <totalsRowFormula>SUMIF(Table327[[#Data],[#Totals],[Movement]],"Credit", Table327[[#Data],[#Totals],[2024-11-01]])-SUMIF(Table327[[#Data],[#Totals],[Movement]],"Debit", Table327[[#Data],[#Totals],[2024-11-01]])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{A7BFC294-B1BF-E445-BCCD-9C9D1112238B}" name="2024-12-01" totalsRowFunction="custom" dataDxfId="98" totalsRowDxfId="0">
+    <tableColumn id="14" xr3:uid="{A7BFC294-B1BF-E445-BCCD-9C9D1112238B}" name="2024-12-01" totalsRowFunction="custom" dataDxfId="98" totalsRowDxfId="10">
       <totalsRowFormula>SUMIF(Table327[[#Data],[#Totals],[Movement]],"Credit", Table327[[#Data],[#Totals],[2024-12-01]])-SUMIF(Table327[[#Data],[#Totals],[Movement]],"Debit", Table327[[#Data],[#Totals],[2024-12-01]])</totalsRowFormula>
     </tableColumn>
   </tableColumns>
@@ -2899,33 +2914,33 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D590EBEC-BC3C-1C40-96B2-E46AB39370B3}" name="Table3272" displayName="Table3272" ref="A1:J7" totalsRowCount="1" headerRowDxfId="97" dataDxfId="96">
-  <autoFilter ref="A1:J6" xr:uid="{92565AF6-51CB-F740-ACD0-AD376C5F8FE0}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D590EBEC-BC3C-1C40-96B2-E46AB39370B3}" name="Table3272" displayName="Table3272" ref="A1:J10" totalsRowCount="1" headerRowDxfId="97" dataDxfId="96">
+  <autoFilter ref="A1:J9" xr:uid="{92565AF6-51CB-F740-ACD0-AD376C5F8FE0}"/>
   <tableColumns count="10">
-    <tableColumn id="5" xr3:uid="{993C14E6-60A9-304A-B4C5-4EBE63033800}" name="Movement" totalsRowLabel="Subtotal" dataDxfId="95" totalsRowDxfId="19"/>
-    <tableColumn id="6" xr3:uid="{A26BC0DA-C92B-4A4A-A60D-1569A7633DC1}" name="Account Secondary" totalsRowLabel="Jodine Transactional" dataDxfId="94" totalsRowDxfId="18"/>
-    <tableColumn id="7" xr3:uid="{4F117689-22E9-4348-A949-D0CA5A13E6B8}" name="2024-05-01" totalsRowFunction="custom" dataDxfId="93" totalsRowDxfId="17">
+    <tableColumn id="5" xr3:uid="{993C14E6-60A9-304A-B4C5-4EBE63033800}" name="Movement" totalsRowLabel="Subtotal" dataDxfId="95" totalsRowDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{A26BC0DA-C92B-4A4A-A60D-1569A7633DC1}" name="Account Secondary" totalsRowLabel="Jodine Transactional" dataDxfId="94" totalsRowDxfId="8"/>
+    <tableColumn id="7" xr3:uid="{4F117689-22E9-4348-A949-D0CA5A13E6B8}" name="2024-05-01" totalsRowFunction="custom" dataDxfId="93" totalsRowDxfId="7">
       <totalsRowFormula>SUMIF(Table3272[[#Data],[#Totals],[Movement]],"Credit", Table3272[[#Data],[#Totals],[2024-05-01]])-SUMIF(Table3272[[#Data],[#Totals],[Movement]],"Debit", Table3272[[#Data],[#Totals],[2024-05-01]])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{4AB7B9EE-431B-8049-81FD-82162F8DB972}" name="2024-06-01" totalsRowFunction="custom" dataDxfId="92" totalsRowDxfId="16">
+    <tableColumn id="8" xr3:uid="{4AB7B9EE-431B-8049-81FD-82162F8DB972}" name="2024-06-01" totalsRowFunction="custom" dataDxfId="92" totalsRowDxfId="6">
       <totalsRowFormula>SUMIF(Table3272[[#Data],[#Totals],[Movement]],"Credit", Table3272[[#Data],[#Totals],[2024-06-01]])-SUMIF(Table3272[[#Data],[#Totals],[Movement]],"Debit", Table3272[[#Data],[#Totals],[2024-06-01]])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{B32522A4-6DB5-0E4B-AEFD-93338290CAD0}" name="2024-07-01" totalsRowFunction="custom" dataDxfId="91" totalsRowDxfId="15">
+    <tableColumn id="9" xr3:uid="{B32522A4-6DB5-0E4B-AEFD-93338290CAD0}" name="2024-07-01" totalsRowFunction="custom" dataDxfId="91" totalsRowDxfId="5">
       <totalsRowFormula>SUMIF(Table3272[[#Data],[#Totals],[Movement]],"Credit", Table3272[[#Data],[#Totals],[2024-07-01]])-SUMIF(Table3272[[#Data],[#Totals],[Movement]],"Debit", Table3272[[#Data],[#Totals],[2024-07-01]])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{4358556B-6A9D-C34C-AEC4-7B51DDFC4B99}" name="2024-08-01" totalsRowFunction="custom" dataDxfId="90" totalsRowDxfId="14">
+    <tableColumn id="10" xr3:uid="{4358556B-6A9D-C34C-AEC4-7B51DDFC4B99}" name="2024-08-01" totalsRowFunction="custom" dataDxfId="90" totalsRowDxfId="4">
       <totalsRowFormula>SUMIF(Table3272[[#Data],[#Totals],[Movement]],"Credit", Table3272[[#Data],[#Totals],[2024-08-01]])-SUMIF(Table3272[[#Data],[#Totals],[Movement]],"Debit", Table3272[[#Data],[#Totals],[2024-08-01]])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{CCFB5DBA-38C3-8748-9ACD-1EE14567004A}" name="2024-09-01" totalsRowFunction="custom" dataDxfId="89" totalsRowDxfId="13">
+    <tableColumn id="11" xr3:uid="{CCFB5DBA-38C3-8748-9ACD-1EE14567004A}" name="2024-09-01" totalsRowFunction="custom" dataDxfId="89" totalsRowDxfId="3">
       <totalsRowFormula>SUMIF(Table3272[[#Data],[#Totals],[Movement]],"Credit", Table3272[[#Data],[#Totals],[2024-09-01]])-SUMIF(Table3272[[#Data],[#Totals],[Movement]],"Debit", Table3272[[#Data],[#Totals],[2024-09-01]])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{178F76AC-AAC4-7A47-BD0E-1401FA1AF282}" name="2024-10-01" totalsRowFunction="custom" dataDxfId="88" totalsRowDxfId="12">
+    <tableColumn id="12" xr3:uid="{178F76AC-AAC4-7A47-BD0E-1401FA1AF282}" name="2024-10-01" totalsRowFunction="custom" dataDxfId="88" totalsRowDxfId="2">
       <totalsRowFormula>SUMIF(Table3272[[#Data],[#Totals],[Movement]],"Credit", Table3272[[#Data],[#Totals],[2024-10-01]])-SUMIF(Table3272[[#Data],[#Totals],[Movement]],"Debit", Table3272[[#Data],[#Totals],[2024-10-01]])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{ED017992-70BF-EA49-8E05-DA8019163116}" name="2024-11-01" totalsRowFunction="custom" dataDxfId="87" totalsRowDxfId="11">
+    <tableColumn id="13" xr3:uid="{ED017992-70BF-EA49-8E05-DA8019163116}" name="2024-11-01" totalsRowFunction="custom" dataDxfId="87" totalsRowDxfId="1">
       <totalsRowFormula>SUMIF(Table3272[[#Data],[#Totals],[Movement]],"Credit", Table3272[[#Data],[#Totals],[2024-11-01]])-SUMIF(Table3272[[#Data],[#Totals],[Movement]],"Debit", Table3272[[#Data],[#Totals],[2024-11-01]])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{5FA47C52-891F-5944-B6FE-936D38AF316E}" name="2024-12-01" totalsRowFunction="custom" dataDxfId="86" totalsRowDxfId="10">
+    <tableColumn id="14" xr3:uid="{5FA47C52-891F-5944-B6FE-936D38AF316E}" name="2024-12-01" totalsRowFunction="custom" dataDxfId="86" totalsRowDxfId="0">
       <totalsRowFormula>SUMIF(Table3272[[#Data],[#Totals],[Movement]],"Credit", Table3272[[#Data],[#Totals],[2024-12-01]])-SUMIF(Table3272[[#Data],[#Totals],[Movement]],"Debit", Table3272[[#Data],[#Totals],[2024-12-01]])</totalsRowFormula>
     </tableColumn>
   </tableColumns>
@@ -2934,33 +2949,33 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{5769C827-0130-1747-96C4-5826BE98F631}" name="Table32734" displayName="Table32734" ref="A1:J7" totalsRowCount="1" headerRowDxfId="63" dataDxfId="62">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{5769C827-0130-1747-96C4-5826BE98F631}" name="Table32734" displayName="Table32734" ref="A1:J7" totalsRowCount="1" headerRowDxfId="85" dataDxfId="84">
   <autoFilter ref="A1:J6" xr:uid="{92565AF6-51CB-F740-ACD0-AD376C5F8FE0}"/>
   <tableColumns count="10">
-    <tableColumn id="5" xr3:uid="{DDD8365D-8383-6844-816A-E3D90FE51FF3}" name="Movement" totalsRowLabel="Subtotal" dataDxfId="61" totalsRowDxfId="51"/>
-    <tableColumn id="6" xr3:uid="{49EDA6C9-9EFA-064E-BCFD-0B004133E7E9}" name="Account Secondary" totalsRowLabel="Jodine Transactional" dataDxfId="60" totalsRowDxfId="50"/>
-    <tableColumn id="7" xr3:uid="{794F9947-7CDA-8F48-9548-050143889B9E}" name="2024-05-01" totalsRowFunction="custom" dataDxfId="59" totalsRowDxfId="49">
+    <tableColumn id="5" xr3:uid="{DDD8365D-8383-6844-816A-E3D90FE51FF3}" name="Movement" totalsRowLabel="Subtotal" dataDxfId="83" totalsRowDxfId="82"/>
+    <tableColumn id="6" xr3:uid="{49EDA6C9-9EFA-064E-BCFD-0B004133E7E9}" name="Account Secondary" totalsRowLabel="Jodine Transactional" dataDxfId="81" totalsRowDxfId="80"/>
+    <tableColumn id="7" xr3:uid="{794F9947-7CDA-8F48-9548-050143889B9E}" name="2024-05-01" totalsRowFunction="custom" dataDxfId="79" totalsRowDxfId="78">
       <totalsRowFormula>SUMIF(Table32734[[#Data],[#Totals],[Movement]],"Credit", Table32734[[#Data],[#Totals],[2024-05-01]])-SUMIF(Table32734[[#Data],[#Totals],[Movement]],"Debit", Table32734[[#Data],[#Totals],[2024-05-01]])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{BBC37A2A-3998-0E42-AFC9-7E88888B1086}" name="2024-06-01" totalsRowFunction="custom" dataDxfId="58" totalsRowDxfId="48">
+    <tableColumn id="8" xr3:uid="{BBC37A2A-3998-0E42-AFC9-7E88888B1086}" name="2024-06-01" totalsRowFunction="custom" dataDxfId="77" totalsRowDxfId="76">
       <totalsRowFormula>SUMIF(Table32734[[#Data],[#Totals],[Movement]],"Credit", Table32734[[#Data],[#Totals],[2024-06-01]])-SUMIF(Table32734[[#Data],[#Totals],[Movement]],"Debit", Table32734[[#Data],[#Totals],[2024-06-01]])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{590C4F00-8EE6-4E46-8DBD-8891F91619E2}" name="2024-07-01" totalsRowFunction="custom" dataDxfId="57" totalsRowDxfId="47">
+    <tableColumn id="9" xr3:uid="{590C4F00-8EE6-4E46-8DBD-8891F91619E2}" name="2024-07-01" totalsRowFunction="custom" dataDxfId="75" totalsRowDxfId="74">
       <totalsRowFormula>SUMIF(Table32734[[#Data],[#Totals],[Movement]],"Credit", Table32734[[#Data],[#Totals],[2024-07-01]])-SUMIF(Table32734[[#Data],[#Totals],[Movement]],"Debit", Table32734[[#Data],[#Totals],[2024-07-01]])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{EFDE75B0-B5DE-F042-BDF0-CD7806088589}" name="2024-08-01" totalsRowFunction="custom" dataDxfId="56" totalsRowDxfId="46">
+    <tableColumn id="10" xr3:uid="{EFDE75B0-B5DE-F042-BDF0-CD7806088589}" name="2024-08-01" totalsRowFunction="custom" dataDxfId="73" totalsRowDxfId="72">
       <totalsRowFormula>SUMIF(Table32734[[#Data],[#Totals],[Movement]],"Credit", Table32734[[#Data],[#Totals],[2024-08-01]])-SUMIF(Table32734[[#Data],[#Totals],[Movement]],"Debit", Table32734[[#Data],[#Totals],[2024-08-01]])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{5C0BE389-226B-9249-A46A-3169D70B574F}" name="2024-09-01" totalsRowFunction="custom" dataDxfId="55" totalsRowDxfId="45">
+    <tableColumn id="11" xr3:uid="{5C0BE389-226B-9249-A46A-3169D70B574F}" name="2024-09-01" totalsRowFunction="custom" dataDxfId="71" totalsRowDxfId="70">
       <totalsRowFormula>SUMIF(Table32734[[#Data],[#Totals],[Movement]],"Credit", Table32734[[#Data],[#Totals],[2024-09-01]])-SUMIF(Table32734[[#Data],[#Totals],[Movement]],"Debit", Table32734[[#Data],[#Totals],[2024-09-01]])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{5DD17303-0F01-294F-9090-E0906189E7DD}" name="2024-10-01" totalsRowFunction="custom" dataDxfId="54" totalsRowDxfId="44">
+    <tableColumn id="12" xr3:uid="{5DD17303-0F01-294F-9090-E0906189E7DD}" name="2024-10-01" totalsRowFunction="custom" dataDxfId="69" totalsRowDxfId="68">
       <totalsRowFormula>SUMIF(Table32734[[#Data],[#Totals],[Movement]],"Credit", Table32734[[#Data],[#Totals],[2024-10-01]])-SUMIF(Table32734[[#Data],[#Totals],[Movement]],"Debit", Table32734[[#Data],[#Totals],[2024-10-01]])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{C691585D-36D3-2C4B-A6D6-4954F2F03EE0}" name="2024-11-01" totalsRowFunction="custom" dataDxfId="53" totalsRowDxfId="43">
+    <tableColumn id="13" xr3:uid="{C691585D-36D3-2C4B-A6D6-4954F2F03EE0}" name="2024-11-01" totalsRowFunction="custom" dataDxfId="67" totalsRowDxfId="66">
       <totalsRowFormula>SUMIF(Table32734[[#Data],[#Totals],[Movement]],"Credit", Table32734[[#Data],[#Totals],[2024-11-01]])-SUMIF(Table32734[[#Data],[#Totals],[Movement]],"Debit", Table32734[[#Data],[#Totals],[2024-11-01]])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{6D41FA26-D619-B14C-8202-960D4BC62D57}" name="2024-12-01" totalsRowFunction="custom" dataDxfId="52" totalsRowDxfId="42">
+    <tableColumn id="14" xr3:uid="{6D41FA26-D619-B14C-8202-960D4BC62D57}" name="2024-12-01" totalsRowFunction="custom" dataDxfId="65" totalsRowDxfId="64">
       <totalsRowFormula>SUMIF(Table32734[[#Data],[#Totals],[Movement]],"Credit", Table32734[[#Data],[#Totals],[2024-12-01]])-SUMIF(Table32734[[#Data],[#Totals],[Movement]],"Debit", Table32734[[#Data],[#Totals],[2024-12-01]])</totalsRowFormula>
     </tableColumn>
   </tableColumns>
@@ -2969,33 +2984,33 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{21F6A830-124F-664D-80AC-384CD45DDB8A}" name="Table32735" displayName="Table32735" ref="A1:J7" totalsRowCount="1" headerRowDxfId="41" dataDxfId="40">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{21F6A830-124F-664D-80AC-384CD45DDB8A}" name="Table32735" displayName="Table32735" ref="A1:J7" totalsRowCount="1" headerRowDxfId="63" dataDxfId="62">
   <autoFilter ref="A1:J6" xr:uid="{92565AF6-51CB-F740-ACD0-AD376C5F8FE0}"/>
   <tableColumns count="10">
-    <tableColumn id="5" xr3:uid="{00DCC526-494A-164C-B8A7-62D8857AA2CC}" name="Movement" totalsRowLabel="Subtotal" dataDxfId="39" totalsRowDxfId="29"/>
-    <tableColumn id="6" xr3:uid="{42900B87-D476-1F4B-B152-C6862D6AD49C}" name="Account Secondary" totalsRowLabel="Jodine Transactional" dataDxfId="38" totalsRowDxfId="28"/>
-    <tableColumn id="7" xr3:uid="{1F324CCC-3D9B-9D43-B1B9-78BC52CEBC4B}" name="2024-05-01" totalsRowFunction="custom" dataDxfId="37" totalsRowDxfId="27">
+    <tableColumn id="5" xr3:uid="{00DCC526-494A-164C-B8A7-62D8857AA2CC}" name="Movement" totalsRowLabel="Subtotal" dataDxfId="61" totalsRowDxfId="60"/>
+    <tableColumn id="6" xr3:uid="{42900B87-D476-1F4B-B152-C6862D6AD49C}" name="Account Secondary" totalsRowLabel="Jodine Transactional" dataDxfId="59" totalsRowDxfId="58"/>
+    <tableColumn id="7" xr3:uid="{1F324CCC-3D9B-9D43-B1B9-78BC52CEBC4B}" name="2024-05-01" totalsRowFunction="custom" dataDxfId="57" totalsRowDxfId="56">
       <totalsRowFormula>SUMIF(Table32735[[#Data],[#Totals],[Movement]],"Credit", Table32735[[#Data],[#Totals],[2024-05-01]])-SUMIF(Table32735[[#Data],[#Totals],[Movement]],"Debit", Table32735[[#Data],[#Totals],[2024-05-01]])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{8D6A0706-954B-6E49-8325-8C5F6C7D0A27}" name="2024-06-01" totalsRowFunction="custom" dataDxfId="36" totalsRowDxfId="26">
+    <tableColumn id="8" xr3:uid="{8D6A0706-954B-6E49-8325-8C5F6C7D0A27}" name="2024-06-01" totalsRowFunction="custom" dataDxfId="55" totalsRowDxfId="54">
       <totalsRowFormula>SUMIF(Table32735[[#Data],[#Totals],[Movement]],"Credit", Table32735[[#Data],[#Totals],[2024-06-01]])-SUMIF(Table32735[[#Data],[#Totals],[Movement]],"Debit", Table32735[[#Data],[#Totals],[2024-06-01]])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{552E7801-D825-E74E-B810-D41F151C53C4}" name="2024-07-01" totalsRowFunction="custom" dataDxfId="35" totalsRowDxfId="25">
+    <tableColumn id="9" xr3:uid="{552E7801-D825-E74E-B810-D41F151C53C4}" name="2024-07-01" totalsRowFunction="custom" dataDxfId="53" totalsRowDxfId="52">
       <totalsRowFormula>SUMIF(Table32735[[#Data],[#Totals],[Movement]],"Credit", Table32735[[#Data],[#Totals],[2024-07-01]])-SUMIF(Table32735[[#Data],[#Totals],[Movement]],"Debit", Table32735[[#Data],[#Totals],[2024-07-01]])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{EC5D0AC7-F33A-904A-8CE5-1901BED12A99}" name="2024-08-01" totalsRowFunction="custom" dataDxfId="34" totalsRowDxfId="24">
+    <tableColumn id="10" xr3:uid="{EC5D0AC7-F33A-904A-8CE5-1901BED12A99}" name="2024-08-01" totalsRowFunction="custom" dataDxfId="51" totalsRowDxfId="50">
       <totalsRowFormula>SUMIF(Table32735[[#Data],[#Totals],[Movement]],"Credit", Table32735[[#Data],[#Totals],[2024-08-01]])-SUMIF(Table32735[[#Data],[#Totals],[Movement]],"Debit", Table32735[[#Data],[#Totals],[2024-08-01]])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{370C335F-82B5-0146-9468-C1048CC4BFF6}" name="2024-09-01" totalsRowFunction="custom" dataDxfId="33" totalsRowDxfId="23">
+    <tableColumn id="11" xr3:uid="{370C335F-82B5-0146-9468-C1048CC4BFF6}" name="2024-09-01" totalsRowFunction="custom" dataDxfId="49" totalsRowDxfId="48">
       <totalsRowFormula>SUMIF(Table32735[[#Data],[#Totals],[Movement]],"Credit", Table32735[[#Data],[#Totals],[2024-09-01]])-SUMIF(Table32735[[#Data],[#Totals],[Movement]],"Debit", Table32735[[#Data],[#Totals],[2024-09-01]])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{91C0D700-3C78-6948-82AE-1144571FA9E0}" name="2024-10-01" totalsRowFunction="custom" dataDxfId="32" totalsRowDxfId="22">
+    <tableColumn id="12" xr3:uid="{91C0D700-3C78-6948-82AE-1144571FA9E0}" name="2024-10-01" totalsRowFunction="custom" dataDxfId="47" totalsRowDxfId="46">
       <totalsRowFormula>SUMIF(Table32735[[#Data],[#Totals],[Movement]],"Credit", Table32735[[#Data],[#Totals],[2024-10-01]])-SUMIF(Table32735[[#Data],[#Totals],[Movement]],"Debit", Table32735[[#Data],[#Totals],[2024-10-01]])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{C6B68C6F-1DB2-BB4C-9DAD-9295D430E9DF}" name="2024-11-01" totalsRowFunction="custom" dataDxfId="31" totalsRowDxfId="21">
+    <tableColumn id="13" xr3:uid="{C6B68C6F-1DB2-BB4C-9DAD-9295D430E9DF}" name="2024-11-01" totalsRowFunction="custom" dataDxfId="45" totalsRowDxfId="44">
       <totalsRowFormula>SUMIF(Table32735[[#Data],[#Totals],[Movement]],"Credit", Table32735[[#Data],[#Totals],[2024-11-01]])-SUMIF(Table32735[[#Data],[#Totals],[Movement]],"Debit", Table32735[[#Data],[#Totals],[2024-11-01]])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{60DA4338-14AB-C441-9F28-1FB5E923B19F}" name="2024-12-01" totalsRowFunction="custom" dataDxfId="30" totalsRowDxfId="20">
+    <tableColumn id="14" xr3:uid="{60DA4338-14AB-C441-9F28-1FB5E923B19F}" name="2024-12-01" totalsRowFunction="custom" dataDxfId="43" totalsRowDxfId="42">
       <totalsRowFormula>SUMIF(Table32735[[#Data],[#Totals],[Movement]],"Credit", Table32735[[#Data],[#Totals],[2024-12-01]])-SUMIF(Table32735[[#Data],[#Totals],[Movement]],"Debit", Table32735[[#Data],[#Totals],[2024-12-01]])</totalsRowFormula>
     </tableColumn>
   </tableColumns>
@@ -3004,33 +3019,33 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{46B86926-7BCD-FD49-A0A1-983772013C0E}" name="Table3273" displayName="Table3273" ref="A1:J7" totalsRowCount="1" headerRowDxfId="85" dataDxfId="84">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{46B86926-7BCD-FD49-A0A1-983772013C0E}" name="Table3273" displayName="Table3273" ref="A1:J7" totalsRowCount="1" headerRowDxfId="41" dataDxfId="40">
   <autoFilter ref="A1:J6" xr:uid="{92565AF6-51CB-F740-ACD0-AD376C5F8FE0}"/>
   <tableColumns count="10">
-    <tableColumn id="5" xr3:uid="{7346A9FB-3ABE-1146-9BF2-50051BE3571E}" name="Movement" totalsRowLabel="Subtotal" dataDxfId="83" totalsRowDxfId="73"/>
-    <tableColumn id="6" xr3:uid="{1A60C668-203A-4643-807D-56767BE2713B}" name="Account Secondary" totalsRowLabel="Jodine Transactional" dataDxfId="82" totalsRowDxfId="72"/>
-    <tableColumn id="7" xr3:uid="{56406242-F73E-D545-871D-CA3D07095EBD}" name="2024-05-01" totalsRowFunction="custom" dataDxfId="81" totalsRowDxfId="71">
+    <tableColumn id="5" xr3:uid="{7346A9FB-3ABE-1146-9BF2-50051BE3571E}" name="Movement" totalsRowLabel="Subtotal" dataDxfId="39" totalsRowDxfId="38"/>
+    <tableColumn id="6" xr3:uid="{1A60C668-203A-4643-807D-56767BE2713B}" name="Account Secondary" totalsRowLabel="Jodine Transactional" dataDxfId="37" totalsRowDxfId="36"/>
+    <tableColumn id="7" xr3:uid="{56406242-F73E-D545-871D-CA3D07095EBD}" name="2024-05-01" totalsRowFunction="custom" dataDxfId="35" totalsRowDxfId="34">
       <totalsRowFormula>SUMIF(Table3273[[#Data],[#Totals],[Movement]],"Credit", Table3273[[#Data],[#Totals],[2024-05-01]])-SUMIF(Table3273[[#Data],[#Totals],[Movement]],"Debit", Table3273[[#Data],[#Totals],[2024-05-01]])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{CEC7C146-DE72-5B45-BB3F-BB9A2B54A98C}" name="2024-06-01" totalsRowFunction="custom" dataDxfId="80" totalsRowDxfId="70">
+    <tableColumn id="8" xr3:uid="{CEC7C146-DE72-5B45-BB3F-BB9A2B54A98C}" name="2024-06-01" totalsRowFunction="custom" dataDxfId="33" totalsRowDxfId="32">
       <totalsRowFormula>SUMIF(Table3273[[#Data],[#Totals],[Movement]],"Credit", Table3273[[#Data],[#Totals],[2024-06-01]])-SUMIF(Table3273[[#Data],[#Totals],[Movement]],"Debit", Table3273[[#Data],[#Totals],[2024-06-01]])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{9FF66E52-7592-8E4A-B720-8102A5B2D81C}" name="2024-07-01" totalsRowFunction="custom" dataDxfId="79" totalsRowDxfId="69">
+    <tableColumn id="9" xr3:uid="{9FF66E52-7592-8E4A-B720-8102A5B2D81C}" name="2024-07-01" totalsRowFunction="custom" dataDxfId="31" totalsRowDxfId="30">
       <totalsRowFormula>SUMIF(Table3273[[#Data],[#Totals],[Movement]],"Credit", Table3273[[#Data],[#Totals],[2024-07-01]])-SUMIF(Table3273[[#Data],[#Totals],[Movement]],"Debit", Table3273[[#Data],[#Totals],[2024-07-01]])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{D9579B17-E722-A54E-86CC-AFD0152C185D}" name="2024-08-01" totalsRowFunction="custom" dataDxfId="78" totalsRowDxfId="68">
+    <tableColumn id="10" xr3:uid="{D9579B17-E722-A54E-86CC-AFD0152C185D}" name="2024-08-01" totalsRowFunction="custom" dataDxfId="29" totalsRowDxfId="28">
       <totalsRowFormula>SUMIF(Table3273[[#Data],[#Totals],[Movement]],"Credit", Table3273[[#Data],[#Totals],[2024-08-01]])-SUMIF(Table3273[[#Data],[#Totals],[Movement]],"Debit", Table3273[[#Data],[#Totals],[2024-08-01]])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{A73CE191-7B1E-734D-B011-77179583A1F9}" name="2024-09-01" totalsRowFunction="custom" dataDxfId="77" totalsRowDxfId="67">
+    <tableColumn id="11" xr3:uid="{A73CE191-7B1E-734D-B011-77179583A1F9}" name="2024-09-01" totalsRowFunction="custom" dataDxfId="27" totalsRowDxfId="26">
       <totalsRowFormula>SUMIF(Table3273[[#Data],[#Totals],[Movement]],"Credit", Table3273[[#Data],[#Totals],[2024-09-01]])-SUMIF(Table3273[[#Data],[#Totals],[Movement]],"Debit", Table3273[[#Data],[#Totals],[2024-09-01]])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{B7E21B7B-8BBD-A44B-A73A-0144E4A44CF0}" name="2024-10-01" totalsRowFunction="custom" dataDxfId="76" totalsRowDxfId="66">
+    <tableColumn id="12" xr3:uid="{B7E21B7B-8BBD-A44B-A73A-0144E4A44CF0}" name="2024-10-01" totalsRowFunction="custom" dataDxfId="25" totalsRowDxfId="24">
       <totalsRowFormula>SUMIF(Table3273[[#Data],[#Totals],[Movement]],"Credit", Table3273[[#Data],[#Totals],[2024-10-01]])-SUMIF(Table3273[[#Data],[#Totals],[Movement]],"Debit", Table3273[[#Data],[#Totals],[2024-10-01]])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{2672CBFB-B3FC-164D-BC7A-B1132CD53672}" name="2024-11-01" totalsRowFunction="custom" dataDxfId="75" totalsRowDxfId="65">
+    <tableColumn id="13" xr3:uid="{2672CBFB-B3FC-164D-BC7A-B1132CD53672}" name="2024-11-01" totalsRowFunction="custom" dataDxfId="23" totalsRowDxfId="22">
       <totalsRowFormula>SUMIF(Table3273[[#Data],[#Totals],[Movement]],"Credit", Table3273[[#Data],[#Totals],[2024-11-01]])-SUMIF(Table3273[[#Data],[#Totals],[Movement]],"Debit", Table3273[[#Data],[#Totals],[2024-11-01]])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{791CE36E-FC3D-404E-857A-3A885BEAD9F9}" name="2024-12-01" totalsRowFunction="custom" dataDxfId="74" totalsRowDxfId="64">
+    <tableColumn id="14" xr3:uid="{791CE36E-FC3D-404E-857A-3A885BEAD9F9}" name="2024-12-01" totalsRowFunction="custom" dataDxfId="21" totalsRowDxfId="20">
       <totalsRowFormula>SUMIF(Table3273[[#Data],[#Totals],[Movement]],"Credit", Table3273[[#Data],[#Totals],[2024-12-01]])-SUMIF(Table3273[[#Data],[#Totals],[Movement]],"Debit", Table3273[[#Data],[#Totals],[2024-12-01]])</totalsRowFormula>
     </tableColumn>
   </tableColumns>
@@ -3357,8 +3372,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5415248B-6FB7-9840-B24A-F55E5AA459E3}">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="L33" sqref="L33"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3414,22 +3429,22 @@
       </c>
       <c r="D2" s="9"/>
       <c r="E2" s="9">
-        <v>2200</v>
+        <v>2500</v>
       </c>
       <c r="F2" s="9">
-        <v>2200</v>
+        <v>2500</v>
       </c>
       <c r="G2" s="9">
-        <v>2200</v>
+        <v>2500</v>
       </c>
       <c r="H2" s="9">
-        <v>2200</v>
+        <v>2500</v>
       </c>
       <c r="I2" s="9">
-        <v>2200</v>
+        <v>2500</v>
       </c>
       <c r="J2" s="9">
-        <v>2200</v>
+        <v>2500</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="3" customFormat="1" ht="22" x14ac:dyDescent="0.3">
@@ -3493,22 +3508,22 @@
       </c>
       <c r="D5" s="12"/>
       <c r="E5" s="12">
-        <v>500</v>
+        <v>750</v>
       </c>
       <c r="F5" s="12">
-        <v>500</v>
+        <v>750</v>
       </c>
       <c r="G5" s="12">
-        <v>500</v>
+        <v>750</v>
       </c>
       <c r="H5" s="12">
-        <v>500</v>
+        <v>750</v>
       </c>
       <c r="I5" s="12">
-        <v>500</v>
+        <v>750</v>
       </c>
       <c r="J5" s="12">
-        <v>500</v>
+        <v>750</v>
       </c>
     </row>
     <row r="6" spans="1:11" s="3" customFormat="1" ht="22" x14ac:dyDescent="0.3">
@@ -3523,22 +3538,22 @@
       </c>
       <c r="D6" s="12"/>
       <c r="E6" s="12">
-        <v>500</v>
+        <v>250</v>
       </c>
       <c r="F6" s="12">
-        <v>500</v>
+        <v>250</v>
       </c>
       <c r="G6" s="12">
-        <v>500</v>
+        <v>250</v>
       </c>
       <c r="H6" s="12">
-        <v>500</v>
+        <v>250</v>
       </c>
       <c r="I6" s="12">
-        <v>500</v>
+        <v>250</v>
       </c>
       <c r="J6" s="12">
-        <v>500</v>
+        <v>250</v>
       </c>
     </row>
     <row r="7" spans="1:11" s="3" customFormat="1" ht="22" x14ac:dyDescent="0.3">
@@ -3550,24 +3565,12 @@
       </c>
       <c r="C7" s="12"/>
       <c r="D7" s="12"/>
-      <c r="E7" s="12">
-        <v>250</v>
-      </c>
-      <c r="F7" s="12">
-        <v>250</v>
-      </c>
-      <c r="G7" s="12">
-        <v>250</v>
-      </c>
-      <c r="H7" s="12">
-        <v>250</v>
-      </c>
-      <c r="I7" s="12">
-        <v>250</v>
-      </c>
-      <c r="J7" s="12">
-        <v>250</v>
-      </c>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
     </row>
     <row r="8" spans="1:11" s="3" customFormat="1" ht="22" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
@@ -3581,22 +3584,22 @@
       </c>
       <c r="D8" s="12"/>
       <c r="E8" s="12">
-        <v>250</v>
+        <v>1000</v>
       </c>
       <c r="F8" s="12">
-        <v>250</v>
+        <v>1000</v>
       </c>
       <c r="G8" s="12">
-        <v>250</v>
+        <v>1000</v>
       </c>
       <c r="H8" s="12">
-        <v>250</v>
+        <v>1000</v>
       </c>
       <c r="I8" s="12">
-        <v>250</v>
+        <v>1000</v>
       </c>
       <c r="J8" s="12">
-        <v>250</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="9" spans="1:11" s="3" customFormat="1" ht="22" x14ac:dyDescent="0.3">
@@ -3652,27 +3655,27 @@
       </c>
       <c r="E11" s="6">
         <f>SUMIF(Table327[[#Data],[#Totals],[Movement]],"Credit", Table327[[#Data],[#Totals],[2024-07-01]])-SUMIF(Table327[[#Data],[#Totals],[Movement]],"Debit", Table327[[#Data],[#Totals],[2024-07-01]])</f>
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="F11" s="6">
         <f>SUMIF(Table327[[#Data],[#Totals],[Movement]],"Credit", Table327[[#Data],[#Totals],[2024-08-01]])-SUMIF(Table327[[#Data],[#Totals],[Movement]],"Debit", Table327[[#Data],[#Totals],[2024-08-01]])</f>
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="G11" s="6">
         <f>SUMIF(Table327[[#Data],[#Totals],[Movement]],"Credit", Table327[[#Data],[#Totals],[2024-09-01]])-SUMIF(Table327[[#Data],[#Totals],[Movement]],"Debit", Table327[[#Data],[#Totals],[2024-09-01]])</f>
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="H11" s="6">
         <f>SUMIF(Table327[[#Data],[#Totals],[Movement]],"Credit", Table327[[#Data],[#Totals],[2024-10-01]])-SUMIF(Table327[[#Data],[#Totals],[Movement]],"Debit", Table327[[#Data],[#Totals],[2024-10-01]])</f>
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="I11" s="6">
         <f>SUMIF(Table327[[#Data],[#Totals],[Movement]],"Credit", Table327[[#Data],[#Totals],[2024-11-01]])-SUMIF(Table327[[#Data],[#Totals],[Movement]],"Debit", Table327[[#Data],[#Totals],[2024-11-01]])</f>
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="J11" s="6">
         <f>SUMIF(Table327[[#Data],[#Totals],[Movement]],"Credit", Table327[[#Data],[#Totals],[2024-12-01]])-SUMIF(Table327[[#Data],[#Totals],[Movement]],"Debit", Table327[[#Data],[#Totals],[2024-12-01]])</f>
-        <v>200</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -3686,10 +3689,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81FC69BB-D6E7-864C-8298-CC4E9A18C604}">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3745,153 +3748,250 @@
       </c>
       <c r="D2" s="9"/>
       <c r="E2" s="9">
-        <v>2000</v>
+        <v>3000</v>
       </c>
       <c r="F2" s="9">
-        <v>2000</v>
+        <v>3000</v>
       </c>
       <c r="G2" s="9">
-        <v>2000</v>
+        <v>3000</v>
       </c>
       <c r="H2" s="9">
-        <v>2000</v>
+        <v>3000</v>
       </c>
       <c r="I2" s="9">
-        <v>2000</v>
+        <v>3000</v>
       </c>
       <c r="J2" s="9">
-        <v>2000</v>
+        <v>3000</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="3" customFormat="1" ht="22" x14ac:dyDescent="0.3">
-      <c r="A3" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="12">
-        <v>0</v>
-      </c>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12">
-        <v>1800</v>
-      </c>
-      <c r="F3" s="12">
-        <v>1800</v>
-      </c>
-      <c r="G3" s="12">
-        <v>1800</v>
-      </c>
-      <c r="H3" s="12">
-        <v>1800</v>
-      </c>
-      <c r="I3" s="12">
-        <v>1800</v>
-      </c>
-      <c r="J3" s="12">
-        <v>1800</v>
-      </c>
-      <c r="K3" s="5"/>
+    <row r="3" spans="1:11" s="2" customFormat="1" ht="22" x14ac:dyDescent="0.3">
+      <c r="A3" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9">
+        <v>1671</v>
+      </c>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
     </row>
     <row r="4" spans="1:11" s="3" customFormat="1" ht="22" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>18</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="C4" s="12">
         <v>0</v>
       </c>
       <c r="D4" s="12"/>
       <c r="E4" s="12">
-        <v>100</v>
+        <v>2000</v>
       </c>
       <c r="F4" s="12">
-        <v>100</v>
+        <v>2000</v>
       </c>
       <c r="G4" s="12">
-        <v>100</v>
+        <v>2000</v>
       </c>
       <c r="H4" s="12">
-        <v>100</v>
+        <v>2000</v>
       </c>
       <c r="I4" s="12">
-        <v>100</v>
+        <v>2000</v>
       </c>
       <c r="J4" s="12">
-        <v>100</v>
-      </c>
+        <v>2000</v>
+      </c>
+      <c r="K4" s="5"/>
     </row>
     <row r="5" spans="1:11" s="3" customFormat="1" ht="22" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="11"/>
-      <c r="C5" s="12"/>
+      <c r="B5" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="12">
+        <v>0</v>
+      </c>
       <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
+      <c r="E5" s="12">
+        <v>200</v>
+      </c>
+      <c r="F5" s="12">
+        <v>200</v>
+      </c>
+      <c r="G5" s="12">
+        <v>200</v>
+      </c>
+      <c r="H5" s="12">
+        <v>200</v>
+      </c>
+      <c r="I5" s="12">
+        <v>200</v>
+      </c>
+      <c r="J5" s="12">
+        <v>200</v>
+      </c>
     </row>
     <row r="6" spans="1:11" s="3" customFormat="1" ht="22" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="12">
+      <c r="B6" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12">
+        <v>500</v>
+      </c>
+      <c r="F6" s="12">
+        <v>500</v>
+      </c>
+      <c r="G6" s="12">
+        <v>500</v>
+      </c>
+      <c r="H6" s="12">
+        <v>500</v>
+      </c>
+      <c r="I6" s="12">
+        <v>500</v>
+      </c>
+      <c r="J6" s="12">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" s="3" customFormat="1" ht="22" x14ac:dyDescent="0.3">
+      <c r="A7" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12">
+        <v>1000</v>
+      </c>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+    </row>
+    <row r="8" spans="1:11" s="3" customFormat="1" ht="22" x14ac:dyDescent="0.3">
+      <c r="A8" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12">
+        <v>200</v>
+      </c>
+      <c r="F8" s="12">
+        <v>200</v>
+      </c>
+      <c r="G8" s="12">
+        <v>200</v>
+      </c>
+      <c r="H8" s="12">
+        <v>200</v>
+      </c>
+      <c r="I8" s="12">
+        <v>200</v>
+      </c>
+      <c r="J8" s="12">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" s="3" customFormat="1" ht="22" x14ac:dyDescent="0.3">
+      <c r="A9" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="12">
         <v>0</v>
       </c>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12">
+        <v>200</v>
+      </c>
+      <c r="F9" s="12">
+        <v>200</v>
+      </c>
+      <c r="G9" s="12">
+        <v>200</v>
+      </c>
+      <c r="H9" s="12">
+        <v>200</v>
+      </c>
+      <c r="I9" s="12">
+        <v>200</v>
+      </c>
+      <c r="J9" s="12">
+        <v>200</v>
+      </c>
     </row>
-    <row r="7" spans="1:11" ht="22" x14ac:dyDescent="0.3">
-      <c r="A7" s="10" t="s">
+    <row r="10" spans="1:11" ht="22" x14ac:dyDescent="0.3">
+      <c r="A10" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B10" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C10" s="6">
         <f>SUMIF(Table3272[[#Data],[#Totals],[Movement]],"Credit", Table3272[[#Data],[#Totals],[2024-05-01]])-SUMIF(Table3272[[#Data],[#Totals],[Movement]],"Debit", Table3272[[#Data],[#Totals],[2024-05-01]])</f>
         <v>0</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D10" s="6">
         <f>SUMIF(Table3272[[#Data],[#Totals],[Movement]],"Credit", Table3272[[#Data],[#Totals],[2024-06-01]])-SUMIF(Table3272[[#Data],[#Totals],[Movement]],"Debit", Table3272[[#Data],[#Totals],[2024-06-01]])</f>
         <v>0</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E10" s="6">
         <f>SUMIF(Table3272[[#Data],[#Totals],[Movement]],"Credit", Table3272[[#Data],[#Totals],[2024-07-01]])-SUMIF(Table3272[[#Data],[#Totals],[Movement]],"Debit", Table3272[[#Data],[#Totals],[2024-07-01]])</f>
-        <v>100</v>
-      </c>
-      <c r="F7" s="6">
+        <v>571</v>
+      </c>
+      <c r="F10" s="6">
         <f>SUMIF(Table3272[[#Data],[#Totals],[Movement]],"Credit", Table3272[[#Data],[#Totals],[2024-08-01]])-SUMIF(Table3272[[#Data],[#Totals],[Movement]],"Debit", Table3272[[#Data],[#Totals],[2024-08-01]])</f>
-        <v>100</v>
-      </c>
-      <c r="G7" s="6">
+        <v>-100</v>
+      </c>
+      <c r="G10" s="6">
         <f>SUMIF(Table3272[[#Data],[#Totals],[Movement]],"Credit", Table3272[[#Data],[#Totals],[2024-09-01]])-SUMIF(Table3272[[#Data],[#Totals],[Movement]],"Debit", Table3272[[#Data],[#Totals],[2024-09-01]])</f>
-        <v>100</v>
-      </c>
-      <c r="H7" s="6">
+        <v>-100</v>
+      </c>
+      <c r="H10" s="6">
         <f>SUMIF(Table3272[[#Data],[#Totals],[Movement]],"Credit", Table3272[[#Data],[#Totals],[2024-10-01]])-SUMIF(Table3272[[#Data],[#Totals],[Movement]],"Debit", Table3272[[#Data],[#Totals],[2024-10-01]])</f>
-        <v>100</v>
-      </c>
-      <c r="I7" s="6">
+        <v>-100</v>
+      </c>
+      <c r="I10" s="6">
         <f>SUMIF(Table3272[[#Data],[#Totals],[Movement]],"Credit", Table3272[[#Data],[#Totals],[2024-11-01]])-SUMIF(Table3272[[#Data],[#Totals],[Movement]],"Debit", Table3272[[#Data],[#Totals],[2024-11-01]])</f>
-        <v>100</v>
-      </c>
-      <c r="J7" s="6">
+        <v>-100</v>
+      </c>
+      <c r="J10" s="6">
         <f>SUMIF(Table3272[[#Data],[#Totals],[Movement]],"Credit", Table3272[[#Data],[#Totals],[2024-12-01]])-SUMIF(Table3272[[#Data],[#Totals],[Movement]],"Debit", Table3272[[#Data],[#Totals],[2024-12-01]])</f>
-        <v>100</v>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="17" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F17" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -4298,7 +4398,7 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="R29" sqref="R29"/>
+      <selection activeCell="AI44" sqref="AI43:AI44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>